<commit_message>
updated reference columns isa.assay
</commit_message>
<xml_diff>
--- a/assays/assay1/isa.assay.xlsx
+++ b/assays/assay1/isa.assay.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/630acb9a9506da97/CSB-Stuff/NFDI/ARC-Hackathon/2021_09/assay_file_for_Hackathon_(ElenaKreis)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\GitHub\Hackathon_SampleRun\assays\assay1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="171" documentId="13_ncr:1_{4D1B671F-397C-462F-BE3F-510DA63CBE77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6295CE74-3F73-41F5-87A4-15D46E372ADF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1A9847-D3F7-4ACE-85F9-D787A8DD5AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plant growth" sheetId="2" r:id="rId1"/>
-    <sheet name="Protein extraction" sheetId="3" r:id="rId2"/>
-    <sheet name="Proteomics MassSpec Assay" sheetId="4" r:id="rId3"/>
-    <sheet name="Proteomics Computational Analys" sheetId="5" r:id="rId4"/>
+    <sheet name="Investigation" sheetId="6" r:id="rId1"/>
+    <sheet name="Plant growth" sheetId="2" r:id="rId2"/>
+    <sheet name="Protein extraction" sheetId="3" r:id="rId3"/>
+    <sheet name="Proteomics MassSpec Assay" sheetId="4" r:id="rId4"/>
+    <sheet name="Proteomics Computational Analys" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="291">
   <si>
     <t>Source Name</t>
   </si>
@@ -861,6 +862,87 @@
   </si>
   <si>
     <t>proteomIqon</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/PECO_0007191</t>
+  </si>
+  <si>
+    <t>Protein extraction</t>
+  </si>
+  <si>
+    <t>minute</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000031</t>
+  </si>
+  <si>
+    <t>ASSAY METADATA</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Comment[&lt;Worksheet&gt;]</t>
+  </si>
+  <si>
+    <t>Roles Term Source REF</t>
+  </si>
+  <si>
+    <t>Roles Term Accession Number</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>Affiliation</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Mid Initials</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>ASSAY PERFORMERS</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Technology Platform</t>
+  </si>
+  <si>
+    <t>Technology Type Term Source REF</t>
+  </si>
+  <si>
+    <t>Technology Type Term Accession Number</t>
+  </si>
+  <si>
+    <t>Technology Type</t>
+  </si>
+  <si>
+    <t>Measurement Type Term Source REF</t>
+  </si>
+  <si>
+    <t>Measurement Type Term Accession Number</t>
+  </si>
+  <si>
+    <t>Measurement Type</t>
   </si>
 </sst>
 </file>
@@ -876,7 +958,7 @@
     <numFmt numFmtId="169" formatCode="0.00\ &quot;minute&quot;"/>
     <numFmt numFmtId="170" formatCode="0.00\ &quot;hour&quot;"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1031,8 +1113,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1218,12 +1307,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor theme="9"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -1364,19 +1447,6 @@
       <left style="thin">
         <color theme="9" tint="0.39997558519241921"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </left>
       <right style="thin">
         <color rgb="FFFFFFFF"/>
       </right>
@@ -1403,8 +1473,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1447,8 +1530,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1486,18 +1570,27 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1532,6 +1625,7 @@
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 2" xfId="42" xr:uid="{75122925-377D-4B10-8A73-00B9D8A51FAD}"/>
     <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1543,60 +1637,6 @@
   </cellStyles>
   <dxfs count="207">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1607,6 +1647,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2075,7 +2124,52 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2195,139 +2289,139 @@
     <tableColumn id="3" xr3:uid="{8AA5043E-A304-4894-B125-6281D52F1ABC}" name="Parameter [Sample storage]" dataDxfId="206"/>
     <tableColumn id="4" xr3:uid="{CDFAB4F2-F532-48DC-B241-50026BC8D8C4}" name="Term Source REF [Sample storage] (#h; #tNFDI4PSO:0000011)" dataDxfId="205"/>
     <tableColumn id="5" xr3:uid="{7CEF2D73-9418-4410-B999-8347AE06252F}" name="Term Accession Number [Sample storage] (#h; #tNFDI4PSO:0000011)" dataDxfId="204"/>
-    <tableColumn id="2" xr3:uid="{5D9E3EF2-8369-49C3-80ED-B17611FF71BD}" name="Unit [degree Celsius] (#3; #h; #tUO:0000027; #u)" dataDxfId="17"/>
-    <tableColumn id="130" xr3:uid="{DDB07F7B-17B7-4A39-9B57-03343C7B6038}" name="Term Source REF [degree Celsius] (#3; #h; #tUO:0000027; #u)" dataDxfId="16"/>
-    <tableColumn id="131" xr3:uid="{A5A078E3-D459-4D53-ACC3-D86D51FECF9A}" name="Term Accession Number [degree Celsius] (#3; #h; #tUO:0000027; #u)" dataDxfId="15"/>
-    <tableColumn id="126" xr3:uid="{706A32EC-AC47-4842-A181-9643A8DA4287}" name="Characteristics [Sample type]" dataDxfId="203"/>
-    <tableColumn id="127" xr3:uid="{AEFE77FC-D63D-4987-BF21-EFEE0C8B1B33}" name="Term Source REF [Sample type] (#h; #tNFDI4PSO:0000064)" dataDxfId="202"/>
-    <tableColumn id="128" xr3:uid="{3B64213D-A010-4184-9DF7-EC9A25D91D65}" name="Term Accession Number [Sample type] (#h; #tNFDI4PSO:0000064)" dataDxfId="201"/>
-    <tableColumn id="123" xr3:uid="{7620DF81-5738-4407-BBC5-C8571DB1BEE4}" name="Characteristics [Biological replicate]" dataDxfId="200"/>
-    <tableColumn id="124" xr3:uid="{B4B57DBB-DE8E-41D0-BB6E-CA582AB9F79C}" name="Term Source REF [Biological replicate] (#h; #tNFDI4PSO:0000042)" dataDxfId="199"/>
-    <tableColumn id="125" xr3:uid="{7D31BFEC-DE18-480B-A046-0EF410C9C6A9}" name="Term Accession Number [Biological replicate] (#h; #tNFDI4PSO:0000042)" dataDxfId="198"/>
-    <tableColumn id="120" xr3:uid="{79E717D0-46B2-4FDF-9997-7837C9F40F3C}" name="Characteristics [Organism]" dataDxfId="197"/>
-    <tableColumn id="121" xr3:uid="{7CC92286-A828-42A8-B7DB-2F7FF8C71C3E}" name="Term Source REF [Organism] (#h; #tNFDI4PSO:0000030)" dataDxfId="196"/>
-    <tableColumn id="122" xr3:uid="{2D24B335-76F1-4F46-A00F-05A1EBC10C80}" name="Term Accession Number [Organism] (#h; #tNFDI4PSO:0000030)" dataDxfId="195"/>
-    <tableColumn id="117" xr3:uid="{5E9F5EE9-2646-4475-BE2B-24A385266D02}" name="Characteristics [Isolate]" dataDxfId="194"/>
-    <tableColumn id="118" xr3:uid="{42DD9E95-B20C-4C50-9568-EF53C71AB53B}" name="Term Source REF [Isolate] (#h; #tNFDI4PSO:0000065)" dataDxfId="193"/>
-    <tableColumn id="119" xr3:uid="{5EAAD5FB-03E8-47D8-9BF6-5A2BC83589BF}" name="Term Accession Number [Isolate] (#h; #tNFDI4PSO:0000065)" dataDxfId="192"/>
-    <tableColumn id="114" xr3:uid="{E40D692E-A32B-4173-9161-8B007F99A647}" name="Characteristics [Cultivar]" dataDxfId="191"/>
-    <tableColumn id="115" xr3:uid="{4A146DE1-6C3D-4054-85DD-B9BE0240E648}" name="Term Source REF [Cultivar] (#h; #tNFDI4PSO:0000066)" dataDxfId="190"/>
-    <tableColumn id="116" xr3:uid="{DC667272-8FA9-40DE-92F7-CB767A5AB55E}" name="Term Accession Number [Cultivar] (#h; #tNFDI4PSO:0000066)" dataDxfId="189"/>
-    <tableColumn id="111" xr3:uid="{470F3907-F895-48C2-84C3-0BD448025911}" name="Characteristics [Ecotype]" dataDxfId="188"/>
-    <tableColumn id="112" xr3:uid="{6571C881-2E0A-4DA1-B476-A4301503B57D}" name="Term Source REF [Ecotype] (#h; #tNFDI4PSO:0000067)" dataDxfId="187"/>
-    <tableColumn id="113" xr3:uid="{CC8F9929-BA1C-42D3-948E-B8048DB7FD48}" name="Term Accession Number [Ecotype] (#h; #tNFDI4PSO:0000067)" dataDxfId="186"/>
-    <tableColumn id="108" xr3:uid="{682FEE54-620E-47E4-A7B5-4FED54E2AF3C}" name="Characteristics [Genotype]" dataDxfId="185"/>
-    <tableColumn id="109" xr3:uid="{A28DB793-D251-482F-98C8-E9CC63452D0A}" name="Term Source REF [Genotype] (#h; #tNFDI4PSO:0000031)" dataDxfId="184"/>
-    <tableColumn id="110" xr3:uid="{12AF6701-1C5F-40F0-9C97-2B29F71F5426}" name="Term Accession Number [Genotype] (#h; #tNFDI4PSO:0000031)" dataDxfId="183"/>
-    <tableColumn id="105" xr3:uid="{CD2C89C4-54A2-42DA-A02A-121F00C10873}" name="Characteristics [population]" dataDxfId="182"/>
-    <tableColumn id="106" xr3:uid="{99EDBBB9-EF8C-4E51-BAD5-EB1D0B3F285C}" name="Term Source REF [population] (#h; #tOBI:0000181)" dataDxfId="181"/>
-    <tableColumn id="107" xr3:uid="{107CB339-ECA0-4D79-81E1-28CD412F9E22}" name="Term Accession Number [population] (#h; #tOBI:0000181)" dataDxfId="180"/>
-    <tableColumn id="102" xr3:uid="{30DBD473-38B0-4E20-8BCC-981C8A619277}" name="Characteristics [Organism part]" dataDxfId="179"/>
-    <tableColumn id="103" xr3:uid="{8EBA3197-6EFA-4128-BDDF-DA8AA206A48A}" name="Term Source REF [Organism part] (#h; #tNFDI4PSO:0000032)" dataDxfId="178"/>
-    <tableColumn id="104" xr3:uid="{D967EFA2-995D-45FA-8F01-6954C66F82FE}" name="Term Accession Number [Organism part] (#h; #tNFDI4PSO:0000032)" dataDxfId="177"/>
-    <tableColumn id="99" xr3:uid="{607FC9EA-B575-4833-A57A-A16EDD62B628}" name="Characteristics [Cell line]" dataDxfId="176"/>
-    <tableColumn id="100" xr3:uid="{05092AC1-1261-4E4F-B561-E3298A766B70}" name="Term Source REF [Cell line] (#h; #tNFDI4PSO:0000068)" dataDxfId="175"/>
-    <tableColumn id="101" xr3:uid="{1E987923-E885-49A3-8E8C-5983E9959614}" name="Term Accession Number [Cell line] (#h; #tNFDI4PSO:0000068)" dataDxfId="174"/>
-    <tableColumn id="96" xr3:uid="{76032110-1F01-4536-8F7F-BD7A1F919633}" name="Characteristics [Cell type]" dataDxfId="173"/>
-    <tableColumn id="97" xr3:uid="{BD69FDBA-6124-4E25-AFAB-C5FAE1CF8BB8}" name="Term Source REF [Cell type] (#h; #tNFDI4PSO:0000069)" dataDxfId="172"/>
-    <tableColumn id="98" xr3:uid="{C368EC75-BC3D-42F9-A69F-8DD153C6F25D}" name="Term Accession Number [Cell type] (#h; #tNFDI4PSO:0000069)" dataDxfId="171"/>
-    <tableColumn id="93" xr3:uid="{59E7AA8E-D325-490D-8A69-CF542C7A59F8}" name="Characteristics [age]" dataDxfId="170"/>
-    <tableColumn id="94" xr3:uid="{0B04E2A2-5BED-46F9-B751-C94C7FE99B8B}" name="Term Source REF [age] (#h; #tNFDI4PSO:0000033)" dataDxfId="169"/>
-    <tableColumn id="95" xr3:uid="{78AE6424-B291-4E11-A546-21AEA37282CE}" name="Term Accession Number [age] (#h; #tNFDI4PSO:0000033)" dataDxfId="168"/>
-    <tableColumn id="90" xr3:uid="{9EF1FC6E-B34F-49D6-B2E0-FBE8382D9D2B}" name="Characteristics [Developmental Stage]" dataDxfId="167"/>
-    <tableColumn id="91" xr3:uid="{D8637FE0-67D8-4C5A-A9A0-CA6ED724FACB}" name="Term Source REF [Developmental Stage] (#h; #tNFDI4PSO:0000070)" dataDxfId="166"/>
-    <tableColumn id="92" xr3:uid="{CD26890F-2BC0-47A1-9351-32D1B49835F0}" name="Term Accession Number [Developmental Stage] (#h; #tNFDI4PSO:0000070)" dataDxfId="165"/>
-    <tableColumn id="87" xr3:uid="{A3E84243-991B-4B5A-8734-B9BFB1D8D061}" name="Characteristics [Plant disease]" dataDxfId="164"/>
-    <tableColumn id="88" xr3:uid="{6AE3C18E-2937-4A02-8937-D43217337F35}" name="Term Source REF [Plant disease] (#h; #tNFDI4PSO:0000071)" dataDxfId="163"/>
-    <tableColumn id="89" xr3:uid="{F0D79F56-6FD0-43CC-AA0D-FFC4724F3F2F}" name="Term Accession Number [Plant disease] (#h; #tNFDI4PSO:0000071)" dataDxfId="162"/>
-    <tableColumn id="84" xr3:uid="{19F11A41-BD19-4763-BE18-E8CDB6BB411C}" name="Characteristics [Plant disease stage]" dataDxfId="161"/>
-    <tableColumn id="85" xr3:uid="{9C7ACE63-3690-4581-95CC-6DFD2EDD6480}" name="Term Source REF [Plant disease stage] (#h; #tNFDI4PSO:0000072)" dataDxfId="160"/>
-    <tableColumn id="86" xr3:uid="{504A06FE-F2D8-4889-83A0-8C0C8FB6065C}" name="Term Accession Number [Plant disease stage] (#h; #tNFDI4PSO:0000072)" dataDxfId="159"/>
-    <tableColumn id="81" xr3:uid="{120171EF-1861-49F1-BE63-53165A4E10BC}" name="Characteristics [Phenotype]" dataDxfId="158"/>
-    <tableColumn id="82" xr3:uid="{0CD65B2D-DEF3-49B9-B79B-206D942E9C89}" name="Term Source REF [Phenotype] (#h; #tNFDI4PSO:0000073)" dataDxfId="157"/>
-    <tableColumn id="83" xr3:uid="{06822785-711C-4DA2-A2A3-2230A0952211}" name="Term Accession Number [Phenotype] (#h; #tNFDI4PSO:0000073)" dataDxfId="156"/>
-    <tableColumn id="78" xr3:uid="{E8C1956B-3CC6-42CF-8EFF-D3940055DA82}" name="Characteristics [whole plant size]" dataDxfId="155"/>
-    <tableColumn id="79" xr3:uid="{5FA98274-6942-4582-8B8B-F58E059B1B09}" name="Term Source REF [whole plant size] (#h; #tTO:1000012)" dataDxfId="154"/>
-    <tableColumn id="80" xr3:uid="{19249EBA-49CA-454C-BA23-786ED3050AA5}" name="Term Accession Number [whole plant size] (#h; #tTO:1000012)" dataDxfId="153"/>
-    <tableColumn id="75" xr3:uid="{496A58D4-784E-4716-A3A9-E37C5CF0A819}" name="Characteristics [study type]" dataDxfId="152"/>
-    <tableColumn id="76" xr3:uid="{8F6D599A-0048-4EB0-B869-ABCE0822B2D7}" name="Term Source REF [study type] (#h; #tPECO:0007231)" dataDxfId="151"/>
-    <tableColumn id="77" xr3:uid="{6A5F3835-936E-439D-8EAB-D8E7EB3E9BBF}" name="Term Accession Number [study type] (#h; #tPECO:0007231)" dataDxfId="150"/>
-    <tableColumn id="72" xr3:uid="{33AD03E9-FC3C-4111-A57B-113AD1FC1FD0}" name="Characteristics [plant growth medium exposure]" dataDxfId="149"/>
-    <tableColumn id="73" xr3:uid="{7103C157-C62A-4B8E-A6AF-8028A18E1BD7}" name="Term Source REF [plant growth medium exposure] (#h; #tPECO:0007147)" dataDxfId="148"/>
-    <tableColumn id="74" xr3:uid="{22B83D36-9739-4454-8DF5-5861846148FB}" name="Term Accession Number [plant growth medium exposure] (#h; #tPECO:0007147)" dataDxfId="147"/>
-    <tableColumn id="69" xr3:uid="{431E4F7A-19D3-4A64-87D1-9A3B238CA8E4}" name="Characteristics [growth plot design]" dataDxfId="146"/>
-    <tableColumn id="70" xr3:uid="{D7C19286-230C-4402-834B-3E6DF3B04FBD}" name="Term Source REF [growth plot design] (#h; #tNFDI4PSO:0000001)" dataDxfId="145"/>
-    <tableColumn id="71" xr3:uid="{00F9020B-D6D3-43F3-8195-8C79E9590AD7}" name="Term Accession Number [growth plot design] (#h; #tNFDI4PSO:0000001)" dataDxfId="144"/>
-    <tableColumn id="66" xr3:uid="{32C38445-730A-4835-9390-DE46C653A550}" name="Characteristics [Growth day length]" dataDxfId="143"/>
-    <tableColumn id="67" xr3:uid="{36141689-EA6E-4BBC-A1FC-CA742C41DCCF}" name="Term Source REF [Growth day length] (#h; #tNFDI4PSO:0000041)" dataDxfId="142"/>
-    <tableColumn id="68" xr3:uid="{87BBACA7-0A84-4A0C-A42F-FDCC8DC54F8F}" name="Term Accession Number [Growth day length] (#h; #tNFDI4PSO:0000041)" dataDxfId="141"/>
-    <tableColumn id="132" xr3:uid="{FED367DE-3D5A-4A91-A597-006E5D1DDED9}" name="Unit [hour] (#h; #tUO:0000032; #u)" dataDxfId="11"/>
-    <tableColumn id="133" xr3:uid="{95FE0D60-D6EF-406B-8BF8-D41C43206511}" name="Term Source REF [hour] (#h; #tUO:0000032; #u)" dataDxfId="10"/>
-    <tableColumn id="134" xr3:uid="{1AC988B5-3475-40E6-91F9-482F4961DD72}" name="Term Accession Number [hour] (#h; #tUO:0000032; #u)" dataDxfId="9"/>
-    <tableColumn id="60" xr3:uid="{79DE72F5-17A8-4D26-BFDF-4D3B929E13E4}" name="Characteristics [light intensity exposure]" dataDxfId="140"/>
-    <tableColumn id="61" xr3:uid="{D625E660-B86B-4459-982B-3D2DCDF073A7}" name="Term Source REF [light intensity exposure] (#h; #tPECO:0007224)" dataDxfId="139"/>
-    <tableColumn id="62" xr3:uid="{4856F0A6-D466-483F-9349-10E7908F515C}" name="Term Accession Number [light intensity exposure] (#h; #tPECO:0007224)" dataDxfId="138"/>
-    <tableColumn id="63" xr3:uid="{CD6441EC-E9D9-4BBE-BCE5-BBA5018B3AF3}" name="Unit [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="137"/>
-    <tableColumn id="64" xr3:uid="{89AF9762-F48B-487B-BD05-4ED8E77A1E73}" name="Term Source REF [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="136"/>
-    <tableColumn id="65" xr3:uid="{17E5CF53-C8FD-446D-8204-971FDF5DFD3A}" name="Term Accession Number [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="135"/>
-    <tableColumn id="54" xr3:uid="{A6513704-7752-42E4-A863-84D24A18BD61}" name="Characteristics [Humidity Day]" dataDxfId="134"/>
-    <tableColumn id="55" xr3:uid="{791A918C-737E-4BF0-AD79-6916B6E13201}" name="Term Source REF [Humidity Day] (#h; #tNFDI4PSO:0000005)" dataDxfId="133"/>
-    <tableColumn id="56" xr3:uid="{E6368113-F948-4075-815D-2AC424B32E3A}" name="Term Accession Number [Humidity Day] (#h; #tNFDI4PSO:0000005)" dataDxfId="132"/>
-    <tableColumn id="57" xr3:uid="{1B37CEF9-335C-4FD9-88C2-48C97172044E}" name="Unit [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="131"/>
-    <tableColumn id="58" xr3:uid="{D9DE516D-A4E6-4A7C-8E7B-14F545CE66A2}" name="Term Source REF [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="130"/>
-    <tableColumn id="59" xr3:uid="{6C50FBA4-7DCA-4448-A9E9-59C5A31F6241}" name="Term Accession Number [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="129"/>
-    <tableColumn id="48" xr3:uid="{B6FF0592-B3D3-4924-BD2F-5CBF5E4E9BBE}" name="Characteristics [Humidity Night]" dataDxfId="128"/>
-    <tableColumn id="49" xr3:uid="{A6EBE56B-C0D1-4CD8-AF80-87963AF9A281}" name="Term Source REF [Humidity Night] (#h; #tNFDI4PSO:0000006)" dataDxfId="127"/>
-    <tableColumn id="50" xr3:uid="{776E4729-0D7F-4E84-B9A9-BA691CDA3383}" name="Term Accession Number [Humidity Night] (#h; #tNFDI4PSO:0000006)" dataDxfId="126"/>
-    <tableColumn id="51" xr3:uid="{B07D3AE3-C0D5-4586-ADC2-90C10CA49034}" name="Unit [percent] (#h; #tUO:0000187; #u)" dataDxfId="125"/>
-    <tableColumn id="52" xr3:uid="{F53339A1-15C8-40E4-BF7C-3AEF2E097425}" name="Term Source REF [percent] (#h; #tUO:0000187; #u)" dataDxfId="124"/>
-    <tableColumn id="53" xr3:uid="{55A3DFC9-C5CA-45FC-8AA3-28CF616F3F14}" name="Term Accession Number [percent] (#h; #tUO:0000187; #u)" dataDxfId="123"/>
-    <tableColumn id="42" xr3:uid="{78B793FE-2E9F-4D84-843B-C202042B633B}" name="Characteristics [Temperature Day]" dataDxfId="122"/>
-    <tableColumn id="43" xr3:uid="{9EE103AF-4199-4161-BEEF-1C52CC80695F}" name="Term Source REF [Temperature Day] (#h; #tNFDI4PSO:0000007)" dataDxfId="121"/>
-    <tableColumn id="44" xr3:uid="{9639FCD5-82C9-49AF-AAA9-B7ED0A3B64F7}" name="Term Accession Number [Temperature Day] (#h; #tNFDI4PSO:0000007)" dataDxfId="120"/>
-    <tableColumn id="45" xr3:uid="{D08DACD5-AE78-408E-8434-8A3F6FAF6344}" name="Unit [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="119"/>
-    <tableColumn id="46" xr3:uid="{CE86C47B-1E20-4231-853F-CB32E512C100}" name="Term Source REF [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="118"/>
-    <tableColumn id="47" xr3:uid="{3D001D71-A7F8-46F5-8C46-FA448945D545}" name="Term Accession Number [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="117"/>
-    <tableColumn id="36" xr3:uid="{32731D3E-0BBF-44F9-B488-9BD66A07BA83}" name="Characteristics [Temperature Night]" dataDxfId="116"/>
-    <tableColumn id="37" xr3:uid="{12F20A47-4CA8-47DE-A142-A933EEB355D3}" name="Term Source REF [Temperature Night] (#h; #tNFDI4PSO:0000008)" dataDxfId="115"/>
-    <tableColumn id="38" xr3:uid="{244204B7-849C-4BC0-94A7-0752AB88064B}" name="Term Accession Number [Temperature Night] (#h; #tNFDI4PSO:0000008)" dataDxfId="114"/>
-    <tableColumn id="39" xr3:uid="{4CE3880B-8212-4801-99F7-9C626815C0F3}" name="Unit [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="113"/>
-    <tableColumn id="40" xr3:uid="{469A0173-6F10-4838-91A2-23DD066A8F99}" name="Term Source REF [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="112"/>
-    <tableColumn id="41" xr3:uid="{759D149E-DC00-4149-86BF-7D207FF65DB1}" name="Term Accession Number [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="111"/>
-    <tableColumn id="33" xr3:uid="{7103EC07-873F-43EC-A6D1-1539827A0F9C}" name="Characteristics [watering exposure]" dataDxfId="110"/>
-    <tableColumn id="34" xr3:uid="{7486597B-F06B-43EE-8EC9-DCEB76929784}" name="Term Source REF [watering exposure] (#h; #tPECO:0007383)" dataDxfId="109"/>
-    <tableColumn id="35" xr3:uid="{0ABD2C9B-9E2B-47AC-A8BB-6E48A5565E25}" name="Term Accession Number [watering exposure] (#h; #tPECO:0007383)" dataDxfId="108"/>
-    <tableColumn id="30" xr3:uid="{ED0A9B4A-AA7B-47B9-81DF-B14002894B8E}" name="Characteristics [plant nutrient exposure]" dataDxfId="107"/>
-    <tableColumn id="31" xr3:uid="{27830A24-0CB9-4578-95CF-91C69A5E9FA9}" name="Term Source REF [plant nutrient exposure] (#h; #tPECO:0007241)" dataDxfId="106"/>
-    <tableColumn id="32" xr3:uid="{BC35A42E-7F2B-4E15-88C1-B2F700B5A6D8}" name="Term Accession Number [plant nutrient exposure] (#h; #tPECO:0007241)" dataDxfId="105"/>
-    <tableColumn id="27" xr3:uid="{529F9FC5-F282-4E20-AB00-0C1CF8DD0CB1}" name="Characteristics [abiotic plant exposure]" dataDxfId="104"/>
-    <tableColumn id="28" xr3:uid="{D1504B59-7C77-4F75-9AD6-5C895B530408}" name="Term Source REF [abiotic plant exposure] (#h; #tPECO:0007191)" dataDxfId="103"/>
-    <tableColumn id="29" xr3:uid="{02F958BF-218E-4799-8168-86100408D972}" name="Term Accession Number [abiotic plant exposure] (#h; #tPECO:0007191)" dataDxfId="102"/>
-    <tableColumn id="135" xr3:uid="{44AD364F-7420-4F84-AAC2-53C7854B3E4B}" name="Unit [degree Celsius] (#h; #u)" dataDxfId="8"/>
-    <tableColumn id="136" xr3:uid="{8E7E3056-8E85-4014-8966-C851B78339E7}" name="Term Source REF [degree Celsius] (#h; #u)" dataDxfId="7"/>
-    <tableColumn id="137" xr3:uid="{9067137A-31D8-421F-827C-547F9A120AC8}" name="Term Accession Number [degree Celsius] (#h; #u)" dataDxfId="6"/>
-    <tableColumn id="24" xr3:uid="{B44B5BCA-5C25-46CF-8A61-3938F5AAE5FC}" name="Characteristics [biotic plant exposure]" dataDxfId="101"/>
-    <tableColumn id="25" xr3:uid="{ECC26870-BF07-43D8-BC35-483993960220}" name="Term Source REF [biotic plant exposure] (#h; #tPECO:0007357)" dataDxfId="100"/>
-    <tableColumn id="26" xr3:uid="{2941B9AC-7A1A-4840-A61D-E8F56B3620E0}" name="Term Accession Number [biotic plant exposure] (#h; #tPECO:0007357)" dataDxfId="99"/>
-    <tableColumn id="21" xr3:uid="{2750D9C8-E906-4386-B4D6-C26DD2A9C610}" name="Characteristics [Geographic Area]" dataDxfId="98"/>
-    <tableColumn id="22" xr3:uid="{6221439A-F035-4331-B264-E65B911B21A2}" name="Term Source REF [Geographic Area] (#h; #tNFDI4PSO:0000074)" dataDxfId="97"/>
-    <tableColumn id="23" xr3:uid="{51F01809-19EF-45D3-A2BB-E3E056D613E1}" name="Term Accession Number [Geographic Area] (#h; #tNFDI4PSO:0000074)" dataDxfId="96"/>
-    <tableColumn id="18" xr3:uid="{55B6F214-4FF2-4696-8AE0-0A0D14B3C803}" name="Characteristics [Sample Collection Date]" dataDxfId="95"/>
-    <tableColumn id="19" xr3:uid="{36E98526-E77C-4E35-82CC-71309A8CEDB3}" name="Term Source REF [Sample Collection Date] (#h; #tNFDI4PSO:0000075)" dataDxfId="94"/>
-    <tableColumn id="20" xr3:uid="{5FFC2C85-D9E0-4D87-ABFE-9265EF15A27D}" name="Term Accession Number [Sample Collection Date] (#h; #tNFDI4PSO:0000075)" dataDxfId="93"/>
-    <tableColumn id="15" xr3:uid="{E62FA0EB-4035-4B55-BEA9-4CD738CF5585}" name="Characteristics [Sample Collected By]" dataDxfId="92"/>
-    <tableColumn id="16" xr3:uid="{F0C67087-6BA4-473B-BDB9-0FD05A167BAA}" name="Term Source REF [Sample Collected By] (#h; #tNFDI4PSO:0000076)" dataDxfId="91"/>
-    <tableColumn id="17" xr3:uid="{66B563F0-CDA0-4BFC-A1B3-7DDFFB31F152}" name="Term Accession Number [Sample Collected By] (#h; #tNFDI4PSO:0000076)" dataDxfId="90"/>
-    <tableColumn id="12" xr3:uid="{1E0B8851-0300-4BCF-908F-F1E239BA49A0}" name="Characteristics [Time point]" dataDxfId="89"/>
-    <tableColumn id="13" xr3:uid="{B47157C3-9DBA-4E30-9E02-AF4E313885DB}" name="Term Source REF [Time point] (#h; #tNFDI4PSO:0000034)" dataDxfId="88"/>
-    <tableColumn id="14" xr3:uid="{EFE4E763-140B-4FB4-8174-3DBD1DD79FE9}" name="Term Accession Number [Time point] (#h; #tNFDI4PSO:0000034)" dataDxfId="87"/>
-    <tableColumn id="9" xr3:uid="{873F5218-8E2B-44ED-B1B8-8761684E6900}" name="Parameter [Sample Collection Method]" dataDxfId="86"/>
-    <tableColumn id="10" xr3:uid="{1B6A3F41-997A-48DF-AA19-1FEF564FD252}" name="Term Source REF [Sample Collection Method] (#h; #tNFDI4PSO:0000009)" dataDxfId="85"/>
-    <tableColumn id="11" xr3:uid="{F081FA15-A513-4E70-9279-6827ABFC54B0}" name="Term Accession Number [Sample Collection Method] (#h; #tNFDI4PSO:0000009)" dataDxfId="84"/>
-    <tableColumn id="6" xr3:uid="{C7628F9A-BDCB-4736-A434-8AC7A2B1081A}" name="Parameter [Metabolism quenching method]" dataDxfId="83"/>
-    <tableColumn id="7" xr3:uid="{6DEB663B-9BE6-46A1-BD8C-F98263EF9E2B}" name="Term Source REF [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)" dataDxfId="82"/>
-    <tableColumn id="8" xr3:uid="{800A08A2-FFEA-4FEF-8356-9C8F98BFD484}" name="Term Accession Number [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)" dataDxfId="81"/>
-    <tableColumn id="129" xr3:uid="{2707AAA0-CCA2-43BE-9C57-DA65D4AFED6F}" name="Sample Name2" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{5D9E3EF2-8369-49C3-80ED-B17611FF71BD}" name="Unit [degree Celsius] (#3; #h; #tUO:0000027; #u)" dataDxfId="203"/>
+    <tableColumn id="130" xr3:uid="{DDB07F7B-17B7-4A39-9B57-03343C7B6038}" name="Term Source REF [degree Celsius] (#3; #h; #tUO:0000027; #u)" dataDxfId="202"/>
+    <tableColumn id="131" xr3:uid="{A5A078E3-D459-4D53-ACC3-D86D51FECF9A}" name="Term Accession Number [degree Celsius] (#3; #h; #tUO:0000027; #u)" dataDxfId="201"/>
+    <tableColumn id="126" xr3:uid="{706A32EC-AC47-4842-A181-9643A8DA4287}" name="Characteristics [Sample type]" dataDxfId="200"/>
+    <tableColumn id="127" xr3:uid="{AEFE77FC-D63D-4987-BF21-EFEE0C8B1B33}" name="Term Source REF [Sample type] (#h; #tNFDI4PSO:0000064)" dataDxfId="199"/>
+    <tableColumn id="128" xr3:uid="{3B64213D-A010-4184-9DF7-EC9A25D91D65}" name="Term Accession Number [Sample type] (#h; #tNFDI4PSO:0000064)" dataDxfId="198"/>
+    <tableColumn id="123" xr3:uid="{7620DF81-5738-4407-BBC5-C8571DB1BEE4}" name="Characteristics [Biological replicate]" dataDxfId="197"/>
+    <tableColumn id="124" xr3:uid="{B4B57DBB-DE8E-41D0-BB6E-CA582AB9F79C}" name="Term Source REF [Biological replicate] (#h; #tNFDI4PSO:0000042)" dataDxfId="196"/>
+    <tableColumn id="125" xr3:uid="{7D31BFEC-DE18-480B-A046-0EF410C9C6A9}" name="Term Accession Number [Biological replicate] (#h; #tNFDI4PSO:0000042)" dataDxfId="195"/>
+    <tableColumn id="120" xr3:uid="{79E717D0-46B2-4FDF-9997-7837C9F40F3C}" name="Characteristics [Organism]" dataDxfId="194"/>
+    <tableColumn id="121" xr3:uid="{7CC92286-A828-42A8-B7DB-2F7FF8C71C3E}" name="Term Source REF [Organism] (#h; #tNFDI4PSO:0000030)" dataDxfId="193"/>
+    <tableColumn id="122" xr3:uid="{2D24B335-76F1-4F46-A00F-05A1EBC10C80}" name="Term Accession Number [Organism] (#h; #tNFDI4PSO:0000030)" dataDxfId="192"/>
+    <tableColumn id="117" xr3:uid="{5E9F5EE9-2646-4475-BE2B-24A385266D02}" name="Characteristics [Isolate]" dataDxfId="191"/>
+    <tableColumn id="118" xr3:uid="{42DD9E95-B20C-4C50-9568-EF53C71AB53B}" name="Term Source REF [Isolate] (#h; #tNFDI4PSO:0000065)" dataDxfId="190"/>
+    <tableColumn id="119" xr3:uid="{5EAAD5FB-03E8-47D8-9BF6-5A2BC83589BF}" name="Term Accession Number [Isolate] (#h; #tNFDI4PSO:0000065)" dataDxfId="189"/>
+    <tableColumn id="114" xr3:uid="{E40D692E-A32B-4173-9161-8B007F99A647}" name="Characteristics [Cultivar]" dataDxfId="188"/>
+    <tableColumn id="115" xr3:uid="{4A146DE1-6C3D-4054-85DD-B9BE0240E648}" name="Term Source REF [Cultivar] (#h; #tNFDI4PSO:0000066)" dataDxfId="187"/>
+    <tableColumn id="116" xr3:uid="{DC667272-8FA9-40DE-92F7-CB767A5AB55E}" name="Term Accession Number [Cultivar] (#h; #tNFDI4PSO:0000066)" dataDxfId="186"/>
+    <tableColumn id="111" xr3:uid="{470F3907-F895-48C2-84C3-0BD448025911}" name="Characteristics [Ecotype]" dataDxfId="185"/>
+    <tableColumn id="112" xr3:uid="{6571C881-2E0A-4DA1-B476-A4301503B57D}" name="Term Source REF [Ecotype] (#h; #tNFDI4PSO:0000067)" dataDxfId="184"/>
+    <tableColumn id="113" xr3:uid="{CC8F9929-BA1C-42D3-948E-B8048DB7FD48}" name="Term Accession Number [Ecotype] (#h; #tNFDI4PSO:0000067)" dataDxfId="183"/>
+    <tableColumn id="108" xr3:uid="{682FEE54-620E-47E4-A7B5-4FED54E2AF3C}" name="Characteristics [Genotype]" dataDxfId="182"/>
+    <tableColumn id="109" xr3:uid="{A28DB793-D251-482F-98C8-E9CC63452D0A}" name="Term Source REF [Genotype] (#h; #tNFDI4PSO:0000031)" dataDxfId="181"/>
+    <tableColumn id="110" xr3:uid="{12AF6701-1C5F-40F0-9C97-2B29F71F5426}" name="Term Accession Number [Genotype] (#h; #tNFDI4PSO:0000031)" dataDxfId="180"/>
+    <tableColumn id="105" xr3:uid="{CD2C89C4-54A2-42DA-A02A-121F00C10873}" name="Characteristics [population]" dataDxfId="179"/>
+    <tableColumn id="106" xr3:uid="{99EDBBB9-EF8C-4E51-BAD5-EB1D0B3F285C}" name="Term Source REF [population] (#h; #tOBI:0000181)" dataDxfId="178"/>
+    <tableColumn id="107" xr3:uid="{107CB339-ECA0-4D79-81E1-28CD412F9E22}" name="Term Accession Number [population] (#h; #tOBI:0000181)" dataDxfId="177"/>
+    <tableColumn id="102" xr3:uid="{30DBD473-38B0-4E20-8BCC-981C8A619277}" name="Characteristics [Organism part]" dataDxfId="176"/>
+    <tableColumn id="103" xr3:uid="{8EBA3197-6EFA-4128-BDDF-DA8AA206A48A}" name="Term Source REF [Organism part] (#h; #tNFDI4PSO:0000032)" dataDxfId="175"/>
+    <tableColumn id="104" xr3:uid="{D967EFA2-995D-45FA-8F01-6954C66F82FE}" name="Term Accession Number [Organism part] (#h; #tNFDI4PSO:0000032)" dataDxfId="174"/>
+    <tableColumn id="99" xr3:uid="{607FC9EA-B575-4833-A57A-A16EDD62B628}" name="Characteristics [Cell line]" dataDxfId="173"/>
+    <tableColumn id="100" xr3:uid="{05092AC1-1261-4E4F-B561-E3298A766B70}" name="Term Source REF [Cell line] (#h; #tNFDI4PSO:0000068)" dataDxfId="172"/>
+    <tableColumn id="101" xr3:uid="{1E987923-E885-49A3-8E8C-5983E9959614}" name="Term Accession Number [Cell line] (#h; #tNFDI4PSO:0000068)" dataDxfId="171"/>
+    <tableColumn id="96" xr3:uid="{76032110-1F01-4536-8F7F-BD7A1F919633}" name="Characteristics [Cell type]" dataDxfId="170"/>
+    <tableColumn id="97" xr3:uid="{BD69FDBA-6124-4E25-AFAB-C5FAE1CF8BB8}" name="Term Source REF [Cell type] (#h; #tNFDI4PSO:0000069)" dataDxfId="169"/>
+    <tableColumn id="98" xr3:uid="{C368EC75-BC3D-42F9-A69F-8DD153C6F25D}" name="Term Accession Number [Cell type] (#h; #tNFDI4PSO:0000069)" dataDxfId="168"/>
+    <tableColumn id="93" xr3:uid="{59E7AA8E-D325-490D-8A69-CF542C7A59F8}" name="Characteristics [age]" dataDxfId="167"/>
+    <tableColumn id="94" xr3:uid="{0B04E2A2-5BED-46F9-B751-C94C7FE99B8B}" name="Term Source REF [age] (#h; #tNFDI4PSO:0000033)" dataDxfId="166"/>
+    <tableColumn id="95" xr3:uid="{78AE6424-B291-4E11-A546-21AEA37282CE}" name="Term Accession Number [age] (#h; #tNFDI4PSO:0000033)" dataDxfId="165"/>
+    <tableColumn id="90" xr3:uid="{9EF1FC6E-B34F-49D6-B2E0-FBE8382D9D2B}" name="Characteristics [Developmental Stage]" dataDxfId="164"/>
+    <tableColumn id="91" xr3:uid="{D8637FE0-67D8-4C5A-A9A0-CA6ED724FACB}" name="Term Source REF [Developmental Stage] (#h; #tNFDI4PSO:0000070)" dataDxfId="163"/>
+    <tableColumn id="92" xr3:uid="{CD26890F-2BC0-47A1-9351-32D1B49835F0}" name="Term Accession Number [Developmental Stage] (#h; #tNFDI4PSO:0000070)" dataDxfId="162"/>
+    <tableColumn id="87" xr3:uid="{A3E84243-991B-4B5A-8734-B9BFB1D8D061}" name="Characteristics [Plant disease]" dataDxfId="161"/>
+    <tableColumn id="88" xr3:uid="{6AE3C18E-2937-4A02-8937-D43217337F35}" name="Term Source REF [Plant disease] (#h; #tNFDI4PSO:0000071)" dataDxfId="160"/>
+    <tableColumn id="89" xr3:uid="{F0D79F56-6FD0-43CC-AA0D-FFC4724F3F2F}" name="Term Accession Number [Plant disease] (#h; #tNFDI4PSO:0000071)" dataDxfId="159"/>
+    <tableColumn id="84" xr3:uid="{19F11A41-BD19-4763-BE18-E8CDB6BB411C}" name="Characteristics [Plant disease stage]" dataDxfId="158"/>
+    <tableColumn id="85" xr3:uid="{9C7ACE63-3690-4581-95CC-6DFD2EDD6480}" name="Term Source REF [Plant disease stage] (#h; #tNFDI4PSO:0000072)" dataDxfId="157"/>
+    <tableColumn id="86" xr3:uid="{504A06FE-F2D8-4889-83A0-8C0C8FB6065C}" name="Term Accession Number [Plant disease stage] (#h; #tNFDI4PSO:0000072)" dataDxfId="156"/>
+    <tableColumn id="81" xr3:uid="{120171EF-1861-49F1-BE63-53165A4E10BC}" name="Characteristics [Phenotype]" dataDxfId="155"/>
+    <tableColumn id="82" xr3:uid="{0CD65B2D-DEF3-49B9-B79B-206D942E9C89}" name="Term Source REF [Phenotype] (#h; #tNFDI4PSO:0000073)" dataDxfId="154"/>
+    <tableColumn id="83" xr3:uid="{06822785-711C-4DA2-A2A3-2230A0952211}" name="Term Accession Number [Phenotype] (#h; #tNFDI4PSO:0000073)" dataDxfId="153"/>
+    <tableColumn id="78" xr3:uid="{E8C1956B-3CC6-42CF-8EFF-D3940055DA82}" name="Characteristics [whole plant size]" dataDxfId="152"/>
+    <tableColumn id="79" xr3:uid="{5FA98274-6942-4582-8B8B-F58E059B1B09}" name="Term Source REF [whole plant size] (#h; #tTO:1000012)" dataDxfId="151"/>
+    <tableColumn id="80" xr3:uid="{19249EBA-49CA-454C-BA23-786ED3050AA5}" name="Term Accession Number [whole plant size] (#h; #tTO:1000012)" dataDxfId="150"/>
+    <tableColumn id="75" xr3:uid="{496A58D4-784E-4716-A3A9-E37C5CF0A819}" name="Characteristics [study type]" dataDxfId="149"/>
+    <tableColumn id="76" xr3:uid="{8F6D599A-0048-4EB0-B869-ABCE0822B2D7}" name="Term Source REF [study type] (#h; #tPECO:0007231)" dataDxfId="148"/>
+    <tableColumn id="77" xr3:uid="{6A5F3835-936E-439D-8EAB-D8E7EB3E9BBF}" name="Term Accession Number [study type] (#h; #tPECO:0007231)" dataDxfId="147"/>
+    <tableColumn id="72" xr3:uid="{33AD03E9-FC3C-4111-A57B-113AD1FC1FD0}" name="Characteristics [plant growth medium exposure]" dataDxfId="146"/>
+    <tableColumn id="73" xr3:uid="{7103C157-C62A-4B8E-A6AF-8028A18E1BD7}" name="Term Source REF [plant growth medium exposure] (#h; #tPECO:0007147)" dataDxfId="145"/>
+    <tableColumn id="74" xr3:uid="{22B83D36-9739-4454-8DF5-5861846148FB}" name="Term Accession Number [plant growth medium exposure] (#h; #tPECO:0007147)" dataDxfId="144"/>
+    <tableColumn id="69" xr3:uid="{431E4F7A-19D3-4A64-87D1-9A3B238CA8E4}" name="Characteristics [growth plot design]" dataDxfId="143"/>
+    <tableColumn id="70" xr3:uid="{D7C19286-230C-4402-834B-3E6DF3B04FBD}" name="Term Source REF [growth plot design] (#h; #tNFDI4PSO:0000001)" dataDxfId="142"/>
+    <tableColumn id="71" xr3:uid="{00F9020B-D6D3-43F3-8195-8C79E9590AD7}" name="Term Accession Number [growth plot design] (#h; #tNFDI4PSO:0000001)" dataDxfId="141"/>
+    <tableColumn id="66" xr3:uid="{32C38445-730A-4835-9390-DE46C653A550}" name="Characteristics [Growth day length]" dataDxfId="140"/>
+    <tableColumn id="67" xr3:uid="{36141689-EA6E-4BBC-A1FC-CA742C41DCCF}" name="Term Source REF [Growth day length] (#h; #tNFDI4PSO:0000041)" dataDxfId="139"/>
+    <tableColumn id="68" xr3:uid="{87BBACA7-0A84-4A0C-A42F-FDCC8DC54F8F}" name="Term Accession Number [Growth day length] (#h; #tNFDI4PSO:0000041)" dataDxfId="138"/>
+    <tableColumn id="132" xr3:uid="{FED367DE-3D5A-4A91-A597-006E5D1DDED9}" name="Unit [hour] (#h; #tUO:0000032; #u)" dataDxfId="137"/>
+    <tableColumn id="133" xr3:uid="{95FE0D60-D6EF-406B-8BF8-D41C43206511}" name="Term Source REF [hour] (#h; #tUO:0000032; #u)" dataDxfId="136"/>
+    <tableColumn id="134" xr3:uid="{1AC988B5-3475-40E6-91F9-482F4961DD72}" name="Term Accession Number [hour] (#h; #tUO:0000032; #u)" dataDxfId="135"/>
+    <tableColumn id="60" xr3:uid="{79DE72F5-17A8-4D26-BFDF-4D3B929E13E4}" name="Characteristics [light intensity exposure]" dataDxfId="134"/>
+    <tableColumn id="61" xr3:uid="{D625E660-B86B-4459-982B-3D2DCDF073A7}" name="Term Source REF [light intensity exposure] (#h; #tPECO:0007224)" dataDxfId="133"/>
+    <tableColumn id="62" xr3:uid="{4856F0A6-D466-483F-9349-10E7908F515C}" name="Term Accession Number [light intensity exposure] (#h; #tPECO:0007224)" dataDxfId="132"/>
+    <tableColumn id="63" xr3:uid="{CD6441EC-E9D9-4BBE-BCE5-BBA5018B3AF3}" name="Unit [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="131"/>
+    <tableColumn id="64" xr3:uid="{89AF9762-F48B-487B-BD05-4ED8E77A1E73}" name="Term Source REF [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="130"/>
+    <tableColumn id="65" xr3:uid="{17E5CF53-C8FD-446D-8204-971FDF5DFD3A}" name="Term Accession Number [microeinstein per square meter per second] (#h; #tUO:0000160; #u)" dataDxfId="129"/>
+    <tableColumn id="54" xr3:uid="{A6513704-7752-42E4-A863-84D24A18BD61}" name="Characteristics [Humidity Day]" dataDxfId="128"/>
+    <tableColumn id="55" xr3:uid="{791A918C-737E-4BF0-AD79-6916B6E13201}" name="Term Source REF [Humidity Day] (#h; #tNFDI4PSO:0000005)" dataDxfId="127"/>
+    <tableColumn id="56" xr3:uid="{E6368113-F948-4075-815D-2AC424B32E3A}" name="Term Accession Number [Humidity Day] (#h; #tNFDI4PSO:0000005)" dataDxfId="126"/>
+    <tableColumn id="57" xr3:uid="{1B37CEF9-335C-4FD9-88C2-48C97172044E}" name="Unit [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="125"/>
+    <tableColumn id="58" xr3:uid="{D9DE516D-A4E6-4A7C-8E7B-14F545CE66A2}" name="Term Source REF [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="124"/>
+    <tableColumn id="59" xr3:uid="{6C50FBA4-7DCA-4448-A9E9-59C5A31F6241}" name="Term Accession Number [percent] (#2; #h; #tUO:0000187; #u)" dataDxfId="123"/>
+    <tableColumn id="48" xr3:uid="{B6FF0592-B3D3-4924-BD2F-5CBF5E4E9BBE}" name="Characteristics [Humidity Night]" dataDxfId="122"/>
+    <tableColumn id="49" xr3:uid="{A6EBE56B-C0D1-4CD8-AF80-87963AF9A281}" name="Term Source REF [Humidity Night] (#h; #tNFDI4PSO:0000006)" dataDxfId="121"/>
+    <tableColumn id="50" xr3:uid="{776E4729-0D7F-4E84-B9A9-BA691CDA3383}" name="Term Accession Number [Humidity Night] (#h; #tNFDI4PSO:0000006)" dataDxfId="120"/>
+    <tableColumn id="51" xr3:uid="{B07D3AE3-C0D5-4586-ADC2-90C10CA49034}" name="Unit [percent] (#h; #tUO:0000187; #u)" dataDxfId="119"/>
+    <tableColumn id="52" xr3:uid="{F53339A1-15C8-40E4-BF7C-3AEF2E097425}" name="Term Source REF [percent] (#h; #tUO:0000187; #u)" dataDxfId="118"/>
+    <tableColumn id="53" xr3:uid="{55A3DFC9-C5CA-45FC-8AA3-28CF616F3F14}" name="Term Accession Number [percent] (#h; #tUO:0000187; #u)" dataDxfId="117"/>
+    <tableColumn id="42" xr3:uid="{78B793FE-2E9F-4D84-843B-C202042B633B}" name="Characteristics [Temperature Day]" dataDxfId="116"/>
+    <tableColumn id="43" xr3:uid="{9EE103AF-4199-4161-BEEF-1C52CC80695F}" name="Term Source REF [Temperature Day] (#h; #tNFDI4PSO:0000007)" dataDxfId="115"/>
+    <tableColumn id="44" xr3:uid="{9639FCD5-82C9-49AF-AAA9-B7ED0A3B64F7}" name="Term Accession Number [Temperature Day] (#h; #tNFDI4PSO:0000007)" dataDxfId="114"/>
+    <tableColumn id="45" xr3:uid="{D08DACD5-AE78-408E-8434-8A3F6FAF6344}" name="Unit [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="113"/>
+    <tableColumn id="46" xr3:uid="{CE86C47B-1E20-4231-853F-CB32E512C100}" name="Term Source REF [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="112"/>
+    <tableColumn id="47" xr3:uid="{3D001D71-A7F8-46F5-8C46-FA448945D545}" name="Term Accession Number [degree Celsius] (#2; #h; #tUO:0000027; #u)" dataDxfId="111"/>
+    <tableColumn id="36" xr3:uid="{32731D3E-0BBF-44F9-B488-9BD66A07BA83}" name="Characteristics [Temperature Night]" dataDxfId="110"/>
+    <tableColumn id="37" xr3:uid="{12F20A47-4CA8-47DE-A142-A933EEB355D3}" name="Term Source REF [Temperature Night] (#h; #tNFDI4PSO:0000008)" dataDxfId="109"/>
+    <tableColumn id="38" xr3:uid="{244204B7-849C-4BC0-94A7-0752AB88064B}" name="Term Accession Number [Temperature Night] (#h; #tNFDI4PSO:0000008)" dataDxfId="108"/>
+    <tableColumn id="39" xr3:uid="{4CE3880B-8212-4801-99F7-9C626815C0F3}" name="Unit [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="107"/>
+    <tableColumn id="40" xr3:uid="{469A0173-6F10-4838-91A2-23DD066A8F99}" name="Term Source REF [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="106"/>
+    <tableColumn id="41" xr3:uid="{759D149E-DC00-4149-86BF-7D207FF65DB1}" name="Term Accession Number [degree Celsius] (#h; #tUO:0000027; #u)" dataDxfId="105"/>
+    <tableColumn id="33" xr3:uid="{7103EC07-873F-43EC-A6D1-1539827A0F9C}" name="Characteristics [watering exposure]" dataDxfId="104"/>
+    <tableColumn id="34" xr3:uid="{7486597B-F06B-43EE-8EC9-DCEB76929784}" name="Term Source REF [watering exposure] (#h; #tPECO:0007383)" dataDxfId="103"/>
+    <tableColumn id="35" xr3:uid="{0ABD2C9B-9E2B-47AC-A8BB-6E48A5565E25}" name="Term Accession Number [watering exposure] (#h; #tPECO:0007383)" dataDxfId="102"/>
+    <tableColumn id="30" xr3:uid="{ED0A9B4A-AA7B-47B9-81DF-B14002894B8E}" name="Characteristics [plant nutrient exposure]" dataDxfId="101"/>
+    <tableColumn id="31" xr3:uid="{27830A24-0CB9-4578-95CF-91C69A5E9FA9}" name="Term Source REF [plant nutrient exposure] (#h; #tPECO:0007241)" dataDxfId="100"/>
+    <tableColumn id="32" xr3:uid="{BC35A42E-7F2B-4E15-88C1-B2F700B5A6D8}" name="Term Accession Number [plant nutrient exposure] (#h; #tPECO:0007241)" dataDxfId="99"/>
+    <tableColumn id="27" xr3:uid="{529F9FC5-F282-4E20-AB00-0C1CF8DD0CB1}" name="Characteristics [abiotic plant exposure]" dataDxfId="98"/>
+    <tableColumn id="28" xr3:uid="{D1504B59-7C77-4F75-9AD6-5C895B530408}" name="Term Source REF [abiotic plant exposure] (#h; #tPECO:0007191)" dataDxfId="97"/>
+    <tableColumn id="29" xr3:uid="{02F958BF-218E-4799-8168-86100408D972}" name="Term Accession Number [abiotic plant exposure] (#h; #tPECO:0007191)" dataDxfId="96"/>
+    <tableColumn id="135" xr3:uid="{44AD364F-7420-4F84-AAC2-53C7854B3E4B}" name="Unit [degree Celsius] (#h; #u)" dataDxfId="95"/>
+    <tableColumn id="136" xr3:uid="{8E7E3056-8E85-4014-8966-C851B78339E7}" name="Term Source REF [degree Celsius] (#h; #u)" dataDxfId="94"/>
+    <tableColumn id="137" xr3:uid="{9067137A-31D8-421F-827C-547F9A120AC8}" name="Term Accession Number [degree Celsius] (#h; #u)" dataDxfId="93"/>
+    <tableColumn id="24" xr3:uid="{B44B5BCA-5C25-46CF-8A61-3938F5AAE5FC}" name="Characteristics [biotic plant exposure]" dataDxfId="92"/>
+    <tableColumn id="25" xr3:uid="{ECC26870-BF07-43D8-BC35-483993960220}" name="Term Source REF [biotic plant exposure] (#h; #tPECO:0007357)" dataDxfId="91"/>
+    <tableColumn id="26" xr3:uid="{2941B9AC-7A1A-4840-A61D-E8F56B3620E0}" name="Term Accession Number [biotic plant exposure] (#h; #tPECO:0007357)" dataDxfId="90"/>
+    <tableColumn id="21" xr3:uid="{2750D9C8-E906-4386-B4D6-C26DD2A9C610}" name="Characteristics [Geographic Area]" dataDxfId="89"/>
+    <tableColumn id="22" xr3:uid="{6221439A-F035-4331-B264-E65B911B21A2}" name="Term Source REF [Geographic Area] (#h; #tNFDI4PSO:0000074)" dataDxfId="88"/>
+    <tableColumn id="23" xr3:uid="{51F01809-19EF-45D3-A2BB-E3E056D613E1}" name="Term Accession Number [Geographic Area] (#h; #tNFDI4PSO:0000074)" dataDxfId="87"/>
+    <tableColumn id="18" xr3:uid="{55B6F214-4FF2-4696-8AE0-0A0D14B3C803}" name="Characteristics [Sample Collection Date]" dataDxfId="86"/>
+    <tableColumn id="19" xr3:uid="{36E98526-E77C-4E35-82CC-71309A8CEDB3}" name="Term Source REF [Sample Collection Date] (#h; #tNFDI4PSO:0000075)" dataDxfId="85"/>
+    <tableColumn id="20" xr3:uid="{5FFC2C85-D9E0-4D87-ABFE-9265EF15A27D}" name="Term Accession Number [Sample Collection Date] (#h; #tNFDI4PSO:0000075)" dataDxfId="84"/>
+    <tableColumn id="15" xr3:uid="{E62FA0EB-4035-4B55-BEA9-4CD738CF5585}" name="Characteristics [Sample Collected By]" dataDxfId="83"/>
+    <tableColumn id="16" xr3:uid="{F0C67087-6BA4-473B-BDB9-0FD05A167BAA}" name="Term Source REF [Sample Collected By] (#h; #tNFDI4PSO:0000076)" dataDxfId="82"/>
+    <tableColumn id="17" xr3:uid="{66B563F0-CDA0-4BFC-A1B3-7DDFFB31F152}" name="Term Accession Number [Sample Collected By] (#h; #tNFDI4PSO:0000076)" dataDxfId="81"/>
+    <tableColumn id="12" xr3:uid="{1E0B8851-0300-4BCF-908F-F1E239BA49A0}" name="Characteristics [Time point]" dataDxfId="80"/>
+    <tableColumn id="13" xr3:uid="{B47157C3-9DBA-4E30-9E02-AF4E313885DB}" name="Term Source REF [Time point] (#h; #tNFDI4PSO:0000034)" dataDxfId="79"/>
+    <tableColumn id="14" xr3:uid="{EFE4E763-140B-4FB4-8174-3DBD1DD79FE9}" name="Term Accession Number [Time point] (#h; #tNFDI4PSO:0000034)" dataDxfId="78"/>
+    <tableColumn id="9" xr3:uid="{873F5218-8E2B-44ED-B1B8-8761684E6900}" name="Parameter [Sample Collection Method]" dataDxfId="77"/>
+    <tableColumn id="10" xr3:uid="{1B6A3F41-997A-48DF-AA19-1FEF564FD252}" name="Term Source REF [Sample Collection Method] (#h; #tNFDI4PSO:0000009)" dataDxfId="76"/>
+    <tableColumn id="11" xr3:uid="{F081FA15-A513-4E70-9279-6827ABFC54B0}" name="Term Accession Number [Sample Collection Method] (#h; #tNFDI4PSO:0000009)" dataDxfId="75"/>
+    <tableColumn id="6" xr3:uid="{C7628F9A-BDCB-4736-A434-8AC7A2B1081A}" name="Parameter [Metabolism quenching method]" dataDxfId="74"/>
+    <tableColumn id="7" xr3:uid="{6DEB663B-9BE6-46A1-BD8C-F98263EF9E2B}" name="Term Source REF [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)" dataDxfId="73"/>
+    <tableColumn id="8" xr3:uid="{800A08A2-FFEA-4FEF-8356-9C8F98BFD484}" name="Term Accession Number [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)" dataDxfId="72"/>
+    <tableColumn id="129" xr3:uid="{2707AAA0-CCA2-43BE-9C57-DA65D4AFED6F}" name="Sample Name2" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2338,34 +2432,34 @@
   <autoFilter ref="A2:AC6" xr:uid="{DFB94463-003D-4301-AEBD-1DFE8D3DCC35}"/>
   <tableColumns count="29">
     <tableColumn id="1" xr3:uid="{67ED7012-64E1-4864-9EBE-9C0FE41A8A35}" name="Source Name"/>
-    <tableColumn id="3" xr3:uid="{C93E6192-8EE8-4F27-BC7B-39F674D917F6}" name="Parameter [protein column]" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{30E9D28D-29C9-44F4-BCAB-EC08D022617B}" name="Term Source REF [protein column] (#h; #tOBI:0000468)" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{EC5C4335-822E-4A59-A322-655DABBA5243}" name="Term Accession Number [protein column] (#h; #tOBI:0000468)" dataDxfId="77"/>
-    <tableColumn id="27" xr3:uid="{139D6030-DABB-4D15-8903-11F468AFDF9B}" name="Parameter [cleavage agent name]" dataDxfId="76"/>
-    <tableColumn id="28" xr3:uid="{DFD04C0F-B399-4C61-8B47-76AFC44E40BD}" name="Term Source REF [cleavage agent name] (#h; #tMS:1001045)" dataDxfId="75"/>
-    <tableColumn id="29" xr3:uid="{E0462116-6C35-4240-9823-9C3CEFD5CD1C}" name="Term Accession Number [cleavage agent name] (#h; #tMS:1001045)" dataDxfId="74"/>
-    <tableColumn id="24" xr3:uid="{3105418C-0C4B-43E1-935E-F19394D1AF32}" name="Parameter [molecule]" dataDxfId="73"/>
-    <tableColumn id="25" xr3:uid="{FF06F47C-F8C9-4312-BF46-EB99C064D947}" name="Term Source REF [molecule] (#h; #tMS:1000859)" dataDxfId="72"/>
-    <tableColumn id="26" xr3:uid="{6AB72219-7201-4063-BD4E-A9C8D6321DAD}" name="Term Accession Number [molecule] (#h; #tMS:1000859)" dataDxfId="71"/>
-    <tableColumn id="21" xr3:uid="{996D05D3-A54A-4014-A4D2-0B8476C99510}" name="Parameter [sample state]" dataDxfId="70"/>
-    <tableColumn id="22" xr3:uid="{4D5D66EA-ED23-4716-9F9B-C47A95129788}" name="Term Source REF [sample state] (#h; #tMS:1000003)" dataDxfId="69"/>
-    <tableColumn id="23" xr3:uid="{E47D54E0-D2DA-41AD-B249-9CAB87F7DC8F}" name="Term Accession Number [sample state] (#h; #tMS:1000003)" dataDxfId="68"/>
-    <tableColumn id="18" xr3:uid="{C00506FF-7A19-4339-B6CF-B7765ACF5318}" name="Parameter [staining]" dataDxfId="67"/>
-    <tableColumn id="19" xr3:uid="{DCA64120-5286-41EC-9C82-CC6BC8DD77FC}" name="Term Source REF [staining] (#h; #tOBI:0302887)" dataDxfId="66"/>
-    <tableColumn id="20" xr3:uid="{2E9B2645-4515-42F0-8DEA-D144AFADDB35}" name="Term Accession Number [staining] (#h; #tOBI:0302887)" dataDxfId="65"/>
-    <tableColumn id="15" xr3:uid="{43B5F1BF-48E8-4D9F-9144-A90920AE6864}" name="Parameter [buffer]" dataDxfId="64"/>
-    <tableColumn id="16" xr3:uid="{13EAC75E-DD41-432B-B885-576880BD64F9}" name="Term Source REF [buffer] (#h; #tCHEBI:35225)" dataDxfId="63"/>
-    <tableColumn id="17" xr3:uid="{715938F7-E7C7-414F-BCFD-23FFB1DF0FDD}" name="Term Accession Number [buffer] (#h; #tCHEBI:35225)" dataDxfId="62"/>
-    <tableColumn id="9" xr3:uid="{D9A5FB79-D6F3-496B-A46E-9B97DF1C3602}" name="Parameter [pH]" dataDxfId="61"/>
-    <tableColumn id="10" xr3:uid="{F8068458-7141-408E-9A00-A85398EB7F4B}" name="Term Source REF [pH] (#h; #tUO:0000196)" dataDxfId="60"/>
-    <tableColumn id="11" xr3:uid="{E09E07E0-4835-463D-A5DF-01237C84C1A0}" name="Term Accession Number [pH] (#h; #tUO:0000196)" dataDxfId="59"/>
-    <tableColumn id="12" xr3:uid="{4A8CA5B9-3C69-4AF4-BF1A-F94155DA2D7C}" name="Unit [pH] (#h; #tUO:0000196; #u)" dataDxfId="58"/>
-    <tableColumn id="13" xr3:uid="{EDA0146D-C8F3-44EE-9964-A499C38102E0}" name="Term Source REF [pH] (#h; #tUO:0000196; #u)" dataDxfId="57"/>
-    <tableColumn id="14" xr3:uid="{081049DA-061C-4E63-B297-5A175C849985}" name="Term Accession Number [pH] (#h; #tUO:0000196; #u)" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{56B6AC34-195E-4095-A0F0-23059B26C54E}" name="Parameter [sample pre-fractionation]" dataDxfId="55"/>
-    <tableColumn id="7" xr3:uid="{B3D5CC79-D678-469F-9729-54184EE8F146}" name="Term Source REF [sample pre-fractionation] (#h; #tMS:1002493)" dataDxfId="54"/>
-    <tableColumn id="8" xr3:uid="{C03EA5DC-31B7-4EBE-B22A-57E52E917FA7}" name="Term Accession Number [sample pre-fractionation] (#h; #tMS:1002493)" dataDxfId="53"/>
-    <tableColumn id="30" xr3:uid="{F45FABA0-671C-4DD9-BDCB-1752468358CE}" name="Sample Name" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{C93E6192-8EE8-4F27-BC7B-39F674D917F6}" name="Parameter [protein column]" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{30E9D28D-29C9-44F4-BCAB-EC08D022617B}" name="Term Source REF [protein column] (#h; #tOBI:0000468)" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{EC5C4335-822E-4A59-A322-655DABBA5243}" name="Term Accession Number [protein column] (#h; #tOBI:0000468)" dataDxfId="68"/>
+    <tableColumn id="27" xr3:uid="{139D6030-DABB-4D15-8903-11F468AFDF9B}" name="Parameter [cleavage agent name]" dataDxfId="67"/>
+    <tableColumn id="28" xr3:uid="{DFD04C0F-B399-4C61-8B47-76AFC44E40BD}" name="Term Source REF [cleavage agent name] (#h; #tMS:1001045)" dataDxfId="66"/>
+    <tableColumn id="29" xr3:uid="{E0462116-6C35-4240-9823-9C3CEFD5CD1C}" name="Term Accession Number [cleavage agent name] (#h; #tMS:1001045)" dataDxfId="65"/>
+    <tableColumn id="24" xr3:uid="{3105418C-0C4B-43E1-935E-F19394D1AF32}" name="Parameter [molecule]" dataDxfId="64"/>
+    <tableColumn id="25" xr3:uid="{FF06F47C-F8C9-4312-BF46-EB99C064D947}" name="Term Source REF [molecule] (#h; #tMS:1000859)" dataDxfId="63"/>
+    <tableColumn id="26" xr3:uid="{6AB72219-7201-4063-BD4E-A9C8D6321DAD}" name="Term Accession Number [molecule] (#h; #tMS:1000859)" dataDxfId="62"/>
+    <tableColumn id="21" xr3:uid="{996D05D3-A54A-4014-A4D2-0B8476C99510}" name="Parameter [sample state]" dataDxfId="61"/>
+    <tableColumn id="22" xr3:uid="{4D5D66EA-ED23-4716-9F9B-C47A95129788}" name="Term Source REF [sample state] (#h; #tMS:1000003)" dataDxfId="60"/>
+    <tableColumn id="23" xr3:uid="{E47D54E0-D2DA-41AD-B249-9CAB87F7DC8F}" name="Term Accession Number [sample state] (#h; #tMS:1000003)" dataDxfId="59"/>
+    <tableColumn id="18" xr3:uid="{C00506FF-7A19-4339-B6CF-B7765ACF5318}" name="Parameter [staining]" dataDxfId="58"/>
+    <tableColumn id="19" xr3:uid="{DCA64120-5286-41EC-9C82-CC6BC8DD77FC}" name="Term Source REF [staining] (#h; #tOBI:0302887)" dataDxfId="57"/>
+    <tableColumn id="20" xr3:uid="{2E9B2645-4515-42F0-8DEA-D144AFADDB35}" name="Term Accession Number [staining] (#h; #tOBI:0302887)" dataDxfId="56"/>
+    <tableColumn id="15" xr3:uid="{43B5F1BF-48E8-4D9F-9144-A90920AE6864}" name="Parameter [buffer]" dataDxfId="55"/>
+    <tableColumn id="16" xr3:uid="{13EAC75E-DD41-432B-B885-576880BD64F9}" name="Term Source REF [buffer] (#h; #tCHEBI:35225)" dataDxfId="54"/>
+    <tableColumn id="17" xr3:uid="{715938F7-E7C7-414F-BCFD-23FFB1DF0FDD}" name="Term Accession Number [buffer] (#h; #tCHEBI:35225)" dataDxfId="53"/>
+    <tableColumn id="9" xr3:uid="{D9A5FB79-D6F3-496B-A46E-9B97DF1C3602}" name="Parameter [pH]" dataDxfId="52"/>
+    <tableColumn id="10" xr3:uid="{F8068458-7141-408E-9A00-A85398EB7F4B}" name="Term Source REF [pH] (#h; #tUO:0000196)" dataDxfId="51"/>
+    <tableColumn id="11" xr3:uid="{E09E07E0-4835-463D-A5DF-01237C84C1A0}" name="Term Accession Number [pH] (#h; #tUO:0000196)" dataDxfId="50"/>
+    <tableColumn id="12" xr3:uid="{4A8CA5B9-3C69-4AF4-BF1A-F94155DA2D7C}" name="Unit [pH] (#h; #tUO:0000196; #u)" dataDxfId="49"/>
+    <tableColumn id="13" xr3:uid="{EDA0146D-C8F3-44EE-9964-A499C38102E0}" name="Term Source REF [pH] (#h; #tUO:0000196; #u)" dataDxfId="48"/>
+    <tableColumn id="14" xr3:uid="{081049DA-061C-4E63-B297-5A175C849985}" name="Term Accession Number [pH] (#h; #tUO:0000196; #u)" dataDxfId="47"/>
+    <tableColumn id="6" xr3:uid="{56B6AC34-195E-4095-A0F0-23059B26C54E}" name="Parameter [sample pre-fractionation]" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{B3D5CC79-D678-469F-9729-54184EE8F146}" name="Term Source REF [sample pre-fractionation] (#h; #tMS:1002493)" dataDxfId="45"/>
+    <tableColumn id="8" xr3:uid="{C03EA5DC-31B7-4EBE-B22A-57E52E917FA7}" name="Term Accession Number [sample pre-fractionation] (#h; #tMS:1002493)" dataDxfId="44"/>
+    <tableColumn id="30" xr3:uid="{F45FABA0-671C-4DD9-BDCB-1752468358CE}" name="Sample Name" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2375,38 +2469,38 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9DCCCA1-9FF5-4AAF-94FE-9C12654CCB10}" name="annotationTable2" displayName="annotationTable2" ref="A2:AF6" totalsRowShown="0">
   <autoFilter ref="A2:AF6" xr:uid="{D9DCCCA1-9FF5-4AAF-94FE-9C12654CCB10}"/>
   <tableColumns count="32">
-    <tableColumn id="1" xr3:uid="{01679849-0FAC-4079-B25B-377C1E5F2E01}" name="Source Name" dataDxfId="51"/>
-    <tableColumn id="31" xr3:uid="{7EA1F89C-A4E5-43EA-B2D2-B235B7C39B07}" name="Parameter [Experiment type]" dataDxfId="50"/>
-    <tableColumn id="32" xr3:uid="{DAE74AD2-259B-4541-8FA0-BDB377A736AA}" name="Term Source REF [Experiment type] (#h; #tPRIDE:0000457)" dataDxfId="49"/>
-    <tableColumn id="33" xr3:uid="{E3267821-FD9F-4A42-AF95-F5D56622A803}" name="Term Accession Number [Experiment type] (#h; #tPRIDE:0000457)" dataDxfId="48"/>
-    <tableColumn id="25" xr3:uid="{5EA49836-7716-4407-A3AE-951AFD0DC082}" name="Parameter [technical replicate]" dataDxfId="47"/>
-    <tableColumn id="26" xr3:uid="{96747230-AD48-4CFD-98E1-C8D2B485327A}" name="Term Source REF [technical replicate] (#h; #tMS:1001808)" dataDxfId="46"/>
-    <tableColumn id="27" xr3:uid="{E79DAB36-4CFA-4809-B7B0-83AAEF98E387}" name="Term Accession Number [technical replicate] (#h; #tMS:1001808)" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{32F3E258-492D-4E08-92AC-4F63996C0539}" name="Parameter [sample volume]" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{F6CFD313-BAFF-40EA-ADD5-261E0F9C185E}" name="Term Source REF [sample volume] (#h; #tMS:1000005)2" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{EB778484-8454-45FE-B10E-816A9317AAE1}" name="Term Accession Number [sample volume] (#h; #tMS:1000005)3" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{43EAEBAE-FB9A-4A72-B21E-D3109120B2CC}" name="Unit [microliter] (#h; #tUO:0000101; #u)" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{3227DADA-407A-4CD0-A7B6-1756D9E6C356}" name="Term Source REF [microliter] (#h; #tUO:0000101; #u)" dataDxfId="40"/>
-    <tableColumn id="10" xr3:uid="{18D34EB9-26E5-4B41-B33D-4FAE46B4B3D3}" name="Term Accession Number [microliter] (#h; #tUO:0000101; #u)" dataDxfId="39"/>
-    <tableColumn id="13" xr3:uid="{80B5FD6D-07D2-41B0-8532-AA7D0057B97D}" name="Parameter [injection volume]" dataDxfId="38"/>
-    <tableColumn id="16" xr3:uid="{4219A834-55F2-42AE-98A9-E6945CA39318}" name="Term Source REF [injection volume] (#h)" dataDxfId="37"/>
-    <tableColumn id="19" xr3:uid="{49A374B2-CFFC-436D-AD8A-619FED254918}" name="Term Accession Number [injection volume] (#h)" dataDxfId="36"/>
-    <tableColumn id="22" xr3:uid="{D7BA6C15-4FC1-4E8E-B60D-B224907C5FF8}" name="Unit [microliter] (#2; #h; #tUO:0000101; #u)" dataDxfId="35"/>
-    <tableColumn id="35" xr3:uid="{881A8F9D-550C-4599-B522-E6EBEB44A5EC}" name="Term Source REF [microliter] (#2; #h; #tUO:0000101; #u)" dataDxfId="34"/>
-    <tableColumn id="36" xr3:uid="{AEF4E107-223B-49C0-A94D-63EEC8B7387A}" name="Term Accession Number [microliter] (#2; #h; #tUO:0000101; #u)" dataDxfId="33"/>
-    <tableColumn id="37" xr3:uid="{1942955B-375E-4D28-8AA7-30DAB4DC4467}" name="Parameter [count unit]" dataDxfId="32"/>
-    <tableColumn id="38" xr3:uid="{F67CC44F-E7CB-4F61-B242-D9AB41DCF29B}" name="Term Source REF [count unit] (#h; #tUO:0000189)4" dataDxfId="31"/>
-    <tableColumn id="39" xr3:uid="{5A84DF1A-739C-4452-9D1E-933AE7F12976}" name="Term Accession Number [count unit] (#h; #tUO:0000189)5" dataDxfId="30"/>
-    <tableColumn id="40" xr3:uid="{53AC95CF-87F0-4A9F-B16C-D3615E945EA2}" name="Parameter [instrument model]" dataDxfId="29"/>
-    <tableColumn id="41" xr3:uid="{994C52F0-29F8-41FB-9176-7148E61FCB5D}" name="Term Source REF [instrument model] (#h; #tMS:1000031)6" dataDxfId="28"/>
-    <tableColumn id="42" xr3:uid="{86784A19-D1BF-42AC-9F8B-EBED15F16B44}" name="Term Accession Number [instrument model] (#h; #tMS:1000031)7" dataDxfId="27"/>
-    <tableColumn id="11" xr3:uid="{EA76AE7F-BD2A-4ED9-939A-92C45CED4689}" name="Parameter [duration]" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{A0BC28D3-5BF2-4F6B-80E4-2BC4064E2FB6}" name="Term Source REF [duration] (#h)" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{759227B5-54C3-4433-9F15-03CA1676E601}" name="Term Accession Number [duration] (#h)" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{FACD2C0B-8515-4B44-9F67-C4D70BF34428}" name="Unit [minute] (#2; #h; #tUO:0000031; #u)" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{1AA3E9F1-CD08-4567-B621-0BF0A6C5BA42}" name="Term Source REF [minute] (#2; #h; #tUO:0000031; #u)" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{1DFE8890-C606-4F97-B7BC-75B4A3CCBB67}" name="Term Accession Number [minute] (#2; #h; #tUO:0000031; #u)" dataDxfId="0"/>
-    <tableColumn id="44" xr3:uid="{6B3F6117-909C-44D0-89DA-AA3539D97840}" name="Data File Name2" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{01679849-0FAC-4079-B25B-377C1E5F2E01}" name="Source Name" dataDxfId="42"/>
+    <tableColumn id="31" xr3:uid="{7EA1F89C-A4E5-43EA-B2D2-B235B7C39B07}" name="Parameter [Experiment type]" dataDxfId="41"/>
+    <tableColumn id="32" xr3:uid="{DAE74AD2-259B-4541-8FA0-BDB377A736AA}" name="Term Source REF [Experiment type] (#h; #tPRIDE:0000457)" dataDxfId="40"/>
+    <tableColumn id="33" xr3:uid="{E3267821-FD9F-4A42-AF95-F5D56622A803}" name="Term Accession Number [Experiment type] (#h; #tPRIDE:0000457)" dataDxfId="39"/>
+    <tableColumn id="25" xr3:uid="{5EA49836-7716-4407-A3AE-951AFD0DC082}" name="Parameter [technical replicate]" dataDxfId="38"/>
+    <tableColumn id="26" xr3:uid="{96747230-AD48-4CFD-98E1-C8D2B485327A}" name="Term Source REF [technical replicate] (#h; #tMS:1001808)" dataDxfId="37"/>
+    <tableColumn id="27" xr3:uid="{E79DAB36-4CFA-4809-B7B0-83AAEF98E387}" name="Term Accession Number [technical replicate] (#h; #tMS:1001808)" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{32F3E258-492D-4E08-92AC-4F63996C0539}" name="Parameter [sample volume]" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{F6CFD313-BAFF-40EA-ADD5-261E0F9C185E}" name="Term Source REF [sample volume] (#h; #tMS:1000005)2" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{EB778484-8454-45FE-B10E-816A9317AAE1}" name="Term Accession Number [sample volume] (#h; #tMS:1000005)3" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{43EAEBAE-FB9A-4A72-B21E-D3109120B2CC}" name="Unit [microliter] (#h; #tUO:0000101; #u)" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{3227DADA-407A-4CD0-A7B6-1756D9E6C356}" name="Term Source REF [microliter] (#h; #tUO:0000101; #u)" dataDxfId="31"/>
+    <tableColumn id="10" xr3:uid="{18D34EB9-26E5-4B41-B33D-4FAE46B4B3D3}" name="Term Accession Number [microliter] (#h; #tUO:0000101; #u)" dataDxfId="30"/>
+    <tableColumn id="13" xr3:uid="{80B5FD6D-07D2-41B0-8532-AA7D0057B97D}" name="Parameter [injection volume]" dataDxfId="29"/>
+    <tableColumn id="16" xr3:uid="{4219A834-55F2-42AE-98A9-E6945CA39318}" name="Term Source REF [injection volume] (#h)" dataDxfId="28"/>
+    <tableColumn id="19" xr3:uid="{49A374B2-CFFC-436D-AD8A-619FED254918}" name="Term Accession Number [injection volume] (#h)" dataDxfId="27"/>
+    <tableColumn id="22" xr3:uid="{D7BA6C15-4FC1-4E8E-B60D-B224907C5FF8}" name="Unit [microliter] (#2; #h; #tUO:0000101; #u)" dataDxfId="26"/>
+    <tableColumn id="35" xr3:uid="{881A8F9D-550C-4599-B522-E6EBEB44A5EC}" name="Term Source REF [microliter] (#2; #h; #tUO:0000101; #u)" dataDxfId="25"/>
+    <tableColumn id="36" xr3:uid="{AEF4E107-223B-49C0-A94D-63EEC8B7387A}" name="Term Accession Number [microliter] (#2; #h; #tUO:0000101; #u)" dataDxfId="24"/>
+    <tableColumn id="37" xr3:uid="{1942955B-375E-4D28-8AA7-30DAB4DC4467}" name="Parameter [count unit]" dataDxfId="23"/>
+    <tableColumn id="38" xr3:uid="{F67CC44F-E7CB-4F61-B242-D9AB41DCF29B}" name="Term Source REF [count unit] (#h; #tUO:0000189)4" dataDxfId="22"/>
+    <tableColumn id="39" xr3:uid="{5A84DF1A-739C-4452-9D1E-933AE7F12976}" name="Term Accession Number [count unit] (#h; #tUO:0000189)5" dataDxfId="21"/>
+    <tableColumn id="40" xr3:uid="{53AC95CF-87F0-4A9F-B16C-D3615E945EA2}" name="Parameter [instrument model]" dataDxfId="20"/>
+    <tableColumn id="41" xr3:uid="{994C52F0-29F8-41FB-9176-7148E61FCB5D}" name="Term Source REF [instrument model] (#h; #tMS:1000031)6" dataDxfId="19"/>
+    <tableColumn id="42" xr3:uid="{86784A19-D1BF-42AC-9F8B-EBED15F16B44}" name="Term Accession Number [instrument model] (#h; #tMS:1000031)7" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{EA76AE7F-BD2A-4ED9-939A-92C45CED4689}" name="Parameter [duration]" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{A0BC28D3-5BF2-4F6B-80E4-2BC4064E2FB6}" name="Term Source REF [duration] (#h)" dataDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{759227B5-54C3-4433-9F15-03CA1676E601}" name="Term Accession Number [duration] (#h)" dataDxfId="15"/>
+    <tableColumn id="15" xr3:uid="{FACD2C0B-8515-4B44-9F67-C4D70BF34428}" name="Unit [minute] (#2; #h; #tUO:0000031; #u)" dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{1AA3E9F1-CD08-4567-B621-0BF0A6C5BA42}" name="Term Source REF [minute] (#2; #h; #tUO:0000031; #u)" dataDxfId="13"/>
+    <tableColumn id="18" xr3:uid="{1DFE8890-C606-4F97-B7BC-75B4A3CCBB67}" name="Term Accession Number [minute] (#2; #h; #tUO:0000031; #u)" dataDxfId="12"/>
+    <tableColumn id="44" xr3:uid="{6B3F6117-909C-44D0-89DA-AA3539D97840}" name="Data File Name2" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2416,17 +2510,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{641CA3EB-C1F6-48ED-981B-DF669F58BE8F}" name="annotationTable3" displayName="annotationTable3" ref="A2:K6" totalsRowShown="0">
   <autoFilter ref="A2:K6" xr:uid="{641CA3EB-C1F6-48ED-981B-DF669F58BE8F}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{C3C09526-F5FD-4147-87B0-F5B36A904537}" name="Source Name" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{58CE0EF0-D629-49BB-9EAD-D6ABB137B49E}" name="Parameter [analysis software]" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{165DFBDF-A7F7-4E65-9E63-73697451E86C}" name="Term Source REF [analysis software] (#h; #tMS:1001456)" dataDxfId="23"/>
-    <tableColumn id="9" xr3:uid="{C582B352-AFA1-44B4-92CA-91D9C722CC16}" name="Term Accession Number [analysis software] (#h; #tMS:1001456)" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{5A06AF7D-8CCA-4180-8EAA-83EBEF421E5F}" name="Parameter [data processing software]" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{8F364E1F-911C-4D72-9056-D9CF662EAF8F}" name="Term Source REF [data processing software] (#h; #tMS:1001457)" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{1F351344-A1B8-4243-927C-6A862D4BE113}" name="Term Accession Number [data processing software] (#h; #tMS:1001457)" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{21162119-28AA-41C4-86F3-48F4CE59986F}" name="Parameter [workflow run]" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{01A24477-682D-46B4-88DE-A09C496E3F13}" name="Term Source REF [workflow run] (#h)" dataDxfId="13"/>
-    <tableColumn id="14" xr3:uid="{66BA9B62-10A5-4BC7-B291-4F71B81494ED}" name="Term Accession Number [workflow run] (#h)" dataDxfId="12"/>
-    <tableColumn id="13" xr3:uid="{F07129CB-D323-43B6-BFE9-1A1E6A053C39}" name="Data File Name2" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{C3C09526-F5FD-4147-87B0-F5B36A904537}" name="Source Name" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{58CE0EF0-D629-49BB-9EAD-D6ABB137B49E}" name="Parameter [analysis software]" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{165DFBDF-A7F7-4E65-9E63-73697451E86C}" name="Term Source REF [analysis software] (#h; #tMS:1001456)" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{C582B352-AFA1-44B4-92CA-91D9C722CC16}" name="Term Accession Number [analysis software] (#h; #tMS:1001456)" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{5A06AF7D-8CCA-4180-8EAA-83EBEF421E5F}" name="Parameter [data processing software]" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{8F364E1F-911C-4D72-9056-D9CF662EAF8F}" name="Term Source REF [data processing software] (#h; #tMS:1001457)" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{1F351344-A1B8-4243-927C-6A862D4BE113}" name="Term Accession Number [data processing software] (#h; #tMS:1001457)" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{21162119-28AA-41C4-86F3-48F4CE59986F}" name="Parameter [workflow run]" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{01A24477-682D-46B4-88DE-A09C496E3F13}" name="Term Source REF [workflow run] (#h)" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{66BA9B62-10A5-4BC7-B291-4F71B81494ED}" name="Term Accession Number [workflow run] (#h)" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{F07129CB-D323-43B6-BFE9-1A1E6A053C39}" name="Data File Name2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2713,7 +2807,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="671" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="1">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -2730,10 +2824,199 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C76375E-62D6-4C51-B928-1A440A0A76F7}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3539CC90-65B0-44DC-841B-FDE74226FC27}">
   <dimension ref="A1:EG74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:EF1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2877,144 +3160,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:137" x14ac:dyDescent="0.25">
-      <c r="A1" s="14"/>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="12"/>
-      <c r="BC1" s="12"/>
-      <c r="BD1" s="12"/>
-      <c r="BE1" s="12"/>
-      <c r="BF1" s="12"/>
-      <c r="BG1" s="12"/>
-      <c r="BH1" s="12"/>
-      <c r="BI1" s="12"/>
-      <c r="BJ1" s="12"/>
-      <c r="BK1" s="12"/>
-      <c r="BL1" s="12"/>
-      <c r="BM1" s="12"/>
-      <c r="BN1" s="12"/>
-      <c r="BO1" s="12"/>
-      <c r="BP1" s="12"/>
-      <c r="BQ1" s="12"/>
-      <c r="BR1" s="12"/>
-      <c r="BS1" s="12"/>
-      <c r="BT1" s="12"/>
-      <c r="BU1" s="12"/>
-      <c r="BV1" s="12"/>
-      <c r="BW1" s="12"/>
-      <c r="BX1" s="12"/>
-      <c r="BY1" s="12"/>
-      <c r="BZ1" s="12"/>
-      <c r="CA1" s="12"/>
-      <c r="CB1" s="12"/>
-      <c r="CC1" s="12"/>
-      <c r="CD1" s="12"/>
-      <c r="CE1" s="12"/>
-      <c r="CF1" s="12"/>
-      <c r="CG1" s="12"/>
-      <c r="CH1" s="12"/>
-      <c r="CI1" s="12"/>
-      <c r="CJ1" s="12"/>
-      <c r="CK1" s="12"/>
-      <c r="CL1" s="12"/>
-      <c r="CM1" s="12"/>
-      <c r="CN1" s="12"/>
-      <c r="CO1" s="12"/>
-      <c r="CP1" s="12"/>
-      <c r="CQ1" s="12"/>
-      <c r="CR1" s="12"/>
-      <c r="CS1" s="12"/>
-      <c r="CT1" s="12"/>
-      <c r="CU1" s="12"/>
-      <c r="CV1" s="12"/>
-      <c r="CW1" s="12"/>
-      <c r="CX1" s="12"/>
-      <c r="CY1" s="12"/>
-      <c r="CZ1" s="12"/>
-      <c r="DA1" s="12"/>
-      <c r="DB1" s="12"/>
-      <c r="DC1" s="12"/>
-      <c r="DD1" s="12"/>
-      <c r="DE1" s="12"/>
-      <c r="DF1" s="12"/>
-      <c r="DG1" s="12"/>
-      <c r="DH1" s="12"/>
-      <c r="DI1" s="12"/>
-      <c r="DJ1" s="12"/>
-      <c r="DK1" s="12"/>
-      <c r="DL1" s="12"/>
-      <c r="DM1" s="12"/>
-      <c r="DN1" s="12"/>
-      <c r="DO1" s="12"/>
-      <c r="DP1" s="12"/>
-      <c r="DQ1" s="12"/>
-      <c r="DR1" s="12"/>
-      <c r="DS1" s="12"/>
-      <c r="DT1" s="12"/>
-      <c r="DU1" s="12"/>
-      <c r="DV1" s="12"/>
-      <c r="DW1" s="12"/>
-      <c r="DX1" s="12"/>
-      <c r="DY1" s="12"/>
-      <c r="DZ1" s="12"/>
-      <c r="EA1" s="12"/>
-      <c r="EB1" s="12"/>
-      <c r="EC1" s="12"/>
-      <c r="ED1" s="12"/>
-      <c r="EE1" s="12"/>
-      <c r="EF1" s="12"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="16"/>
+      <c r="AM1" s="16"/>
+      <c r="AN1" s="16"/>
+      <c r="AO1" s="16"/>
+      <c r="AP1" s="16"/>
+      <c r="AQ1" s="16"/>
+      <c r="AR1" s="16"/>
+      <c r="AS1" s="16"/>
+      <c r="AT1" s="16"/>
+      <c r="AU1" s="16"/>
+      <c r="AV1" s="16"/>
+      <c r="AW1" s="16"/>
+      <c r="AX1" s="16"/>
+      <c r="AY1" s="16"/>
+      <c r="AZ1" s="16"/>
+      <c r="BA1" s="16"/>
+      <c r="BB1" s="16"/>
+      <c r="BC1" s="16"/>
+      <c r="BD1" s="16"/>
+      <c r="BE1" s="16"/>
+      <c r="BF1" s="16"/>
+      <c r="BG1" s="16"/>
+      <c r="BH1" s="16"/>
+      <c r="BI1" s="16"/>
+      <c r="BJ1" s="16"/>
+      <c r="BK1" s="16"/>
+      <c r="BL1" s="16"/>
+      <c r="BM1" s="16"/>
+      <c r="BN1" s="16"/>
+      <c r="BO1" s="16"/>
+      <c r="BP1" s="16"/>
+      <c r="BQ1" s="16"/>
+      <c r="BR1" s="16"/>
+      <c r="BS1" s="16"/>
+      <c r="BT1" s="16"/>
+      <c r="BU1" s="16"/>
+      <c r="BV1" s="16"/>
+      <c r="BW1" s="16"/>
+      <c r="BX1" s="16"/>
+      <c r="BY1" s="16"/>
+      <c r="BZ1" s="16"/>
+      <c r="CA1" s="16"/>
+      <c r="CB1" s="16"/>
+      <c r="CC1" s="16"/>
+      <c r="CD1" s="16"/>
+      <c r="CE1" s="16"/>
+      <c r="CF1" s="16"/>
+      <c r="CG1" s="16"/>
+      <c r="CH1" s="16"/>
+      <c r="CI1" s="16"/>
+      <c r="CJ1" s="16"/>
+      <c r="CK1" s="16"/>
+      <c r="CL1" s="16"/>
+      <c r="CM1" s="16"/>
+      <c r="CN1" s="16"/>
+      <c r="CO1" s="16"/>
+      <c r="CP1" s="16"/>
+      <c r="CQ1" s="16"/>
+      <c r="CR1" s="16"/>
+      <c r="CS1" s="16"/>
+      <c r="CT1" s="16"/>
+      <c r="CU1" s="16"/>
+      <c r="CV1" s="16"/>
+      <c r="CW1" s="16"/>
+      <c r="CX1" s="16"/>
+      <c r="CY1" s="16"/>
+      <c r="CZ1" s="16"/>
+      <c r="DA1" s="16"/>
+      <c r="DB1" s="16"/>
+      <c r="DC1" s="16"/>
+      <c r="DD1" s="16"/>
+      <c r="DE1" s="16"/>
+      <c r="DF1" s="16"/>
+      <c r="DG1" s="16"/>
+      <c r="DH1" s="16"/>
+      <c r="DI1" s="16"/>
+      <c r="DJ1" s="16"/>
+      <c r="DK1" s="16"/>
+      <c r="DL1" s="16"/>
+      <c r="DM1" s="16"/>
+      <c r="DN1" s="16"/>
+      <c r="DO1" s="16"/>
+      <c r="DP1" s="16"/>
+      <c r="DQ1" s="16"/>
+      <c r="DR1" s="16"/>
+      <c r="DS1" s="16"/>
+      <c r="DT1" s="16"/>
+      <c r="DU1" s="16"/>
+      <c r="DV1" s="16"/>
+      <c r="DW1" s="16"/>
+      <c r="DX1" s="16"/>
+      <c r="DY1" s="16"/>
+      <c r="DZ1" s="16"/>
+      <c r="EA1" s="16"/>
+      <c r="EB1" s="16"/>
+      <c r="EC1" s="16"/>
+      <c r="ED1" s="16"/>
+      <c r="EE1" s="16"/>
+      <c r="EF1" s="16"/>
       <c r="EG1" s="11"/>
     </row>
     <row r="2" spans="1:137" x14ac:dyDescent="0.25">
@@ -3560,7 +3843,7 @@
       <c r="BM3" s="2"/>
       <c r="BN3" s="1"/>
       <c r="BO3" s="1"/>
-      <c r="BP3" s="16">
+      <c r="BP3" s="15">
         <v>24</v>
       </c>
       <c r="BQ3" s="1" t="s">
@@ -3670,14 +3953,20 @@
         <v>25</v>
       </c>
       <c r="DG3" s="1" t="s">
-        <v>197</v>
+        <v>230</v>
       </c>
       <c r="DH3" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="DI3" s="1"/>
-      <c r="DJ3" s="1"/>
-      <c r="DK3" s="1"/>
+        <v>264</v>
+      </c>
+      <c r="DI3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="DJ3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="DK3" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="DL3" s="2"/>
       <c r="DM3" s="1"/>
       <c r="DN3" s="1"/>
@@ -3857,7 +4146,7 @@
       <c r="BM4" s="2"/>
       <c r="BN4" s="1"/>
       <c r="BO4" s="1"/>
-      <c r="BP4" s="16">
+      <c r="BP4" s="15">
         <v>24</v>
       </c>
       <c r="BQ4" s="1" t="s">
@@ -3967,14 +4256,20 @@
         <v>25</v>
       </c>
       <c r="DG4" s="1" t="s">
-        <v>197</v>
+        <v>230</v>
       </c>
       <c r="DH4" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="DI4" s="1"/>
-      <c r="DJ4" s="1"/>
-      <c r="DK4" s="1"/>
+        <v>264</v>
+      </c>
+      <c r="DI4" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="DJ4" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="DK4" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="DL4" s="2"/>
       <c r="DM4" s="1"/>
       <c r="DN4" s="1"/>
@@ -4154,7 +4449,7 @@
       <c r="BM5" s="2"/>
       <c r="BN5" s="1"/>
       <c r="BO5" s="1"/>
-      <c r="BP5" s="16">
+      <c r="BP5" s="15">
         <v>24</v>
       </c>
       <c r="BQ5" s="1" t="s">
@@ -4264,14 +4559,20 @@
         <v>25</v>
       </c>
       <c r="DG5" s="1" t="s">
-        <v>197</v>
+        <v>230</v>
       </c>
       <c r="DH5" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="DI5" s="1"/>
-      <c r="DJ5" s="1"/>
-      <c r="DK5" s="1"/>
+        <v>264</v>
+      </c>
+      <c r="DI5" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="DJ5" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="DK5" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="DL5" s="2"/>
       <c r="DM5" s="1"/>
       <c r="DN5" s="1"/>
@@ -4451,7 +4752,7 @@
       <c r="BM6" s="2"/>
       <c r="BN6" s="1"/>
       <c r="BO6" s="1"/>
-      <c r="BP6" s="16">
+      <c r="BP6" s="15">
         <v>24</v>
       </c>
       <c r="BQ6" s="1" t="s">
@@ -4561,14 +4862,20 @@
         <v>25</v>
       </c>
       <c r="DG6" s="1" t="s">
-        <v>197</v>
+        <v>230</v>
       </c>
       <c r="DH6" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="DI6" s="1"/>
-      <c r="DJ6" s="1"/>
-      <c r="DK6" s="1"/>
+        <v>264</v>
+      </c>
+      <c r="DI6" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="DJ6" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="DK6" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="DL6" s="2"/>
       <c r="DM6" s="1"/>
       <c r="DN6" s="1"/>
@@ -7202,7 +7509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71670B6D-3609-4CAB-A895-7CD6757FCFFD}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
@@ -7243,34 +7550,36 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
+      <c r="B1" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="18"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -7662,6 +7971,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:AB1"/>
+  </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -7670,9 +7982,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E4D613-0E48-439D-8F94-D255EC84400F}">
-  <dimension ref="A1:AH26"/>
+  <dimension ref="A1:AF26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7713,37 +8025,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A1" s="14"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
+      <c r="A1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
       <c r="AF1" s="11"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -7923,9 +8235,15 @@
       <c r="AB3" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
+      <c r="AC3" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="AF3" s="2" t="s">
         <v>221</v>
       </c>
@@ -8009,9 +8327,15 @@
       <c r="AB4" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
+      <c r="AC4" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="AF4" s="2" t="s">
         <v>220</v>
       </c>
@@ -8095,9 +8419,15 @@
       <c r="AB5" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
+      <c r="AC5" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="AF5" s="2" t="s">
         <v>222</v>
       </c>
@@ -8181,9 +8511,15 @@
       <c r="AB6" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
+      <c r="AC6" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="AF6" s="2" t="s">
         <v>223</v>
       </c>
@@ -8358,7 +8694,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790FF081-8EEF-4D4E-9888-950BE7847F39}">
   <dimension ref="A1:M26"/>
   <sheetViews>
@@ -8383,17 +8719,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="14"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="A1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
     </row>

</xml_diff>